<commit_message>
Add tencent cloud API for user management and face search.
</commit_message>
<xml_diff>
--- a/namelist.xlsx
+++ b/namelist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junxianshen/Documents/programs/python/face_recognition/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saya\Desktop\qrcode-face_recog_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FBD061-6A17-D245-B0A8-B89E0206F66F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD86626-D13D-4DEE-9359-3CCE9B2B8E69}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19020" yWindow="1720" windowWidth="28240" windowHeight="17440" xr2:uid="{2DBE1D61-800C-B944-A68B-CC5700C58460}"/>
+    <workbookView xWindow="4890" yWindow="5115" windowWidth="28800" windowHeight="15885" xr2:uid="{2DBE1D61-800C-B944-A68B-CC5700C58460}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>姓名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>范英晨</t>
+  </si>
+  <si>
+    <t>王敏虎</t>
   </si>
 </sst>
 </file>
@@ -142,14 +145,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -157,7 +160,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -165,7 +168,7 @@
     <font>
       <sz val="13"/>
       <color rgb="FF000000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -205,7 +208,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -221,7 +224,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -517,13 +520,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A51026-8F54-DA44-B617-A63FA1BB182E}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -555,7 +558,7 @@
         <v>2019214570</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17">
+    <row r="4" spans="1:3" ht="17.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -571,7 +574,7 @@
         <v>2019214562</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17">
+    <row r="6" spans="1:3" ht="17.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -579,7 +582,7 @@
         <v>2019312681</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17">
+    <row r="7" spans="1:3" ht="17.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -587,7 +590,7 @@
         <v>2019214557</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17">
+    <row r="8" spans="1:3" ht="17.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -753,6 +756,14 @@
       </c>
       <c r="B28">
         <v>2019214571</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29">
+        <v>2019312688</v>
       </c>
     </row>
   </sheetData>

</xml_diff>